<commit_message>
Country changes, predict_f --> predict_y, mobility excel changes, csv tables for all notebooks, kernel analysis
</commit_message>
<xml_diff>
--- a/Data/Population/Data_Extract_From_World_Development_Indicators.xlsx
+++ b/Data/Population/Data_Extract_From_World_Development_Indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgios\Desktop\GitHub\COVID\gp-george\compartmental-epidemic-model\Data\Population\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgios\Desktop\GitHub\COVID\final-gp\epidemic-gaussian-process\Data\Population\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A368FE-34B9-4576-96A9-5944E12E5419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836638A3-D108-4974-BF86-91C7ABFD219C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23565" yWindow="5475" windowWidth="15600" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="19275" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>Aggregation method</t>
   </si>
   <si>
-    <t>South Africa</t>
-  </si>
-  <si>
     <t>Thailand</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>Last Updated: 10/13/2020</t>
   </si>
   <si>
-    <t>Algeria</t>
-  </si>
-  <si>
     <t>Turkey</t>
   </si>
   <si>
@@ -161,6 +155,12 @@
   </si>
   <si>
     <t>Egypt</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Kenya</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,21 +515,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
       <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>53734979</v>
@@ -544,7 +544,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>75032834</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>37330545</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>214146999</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>38482525</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>28833291</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>55883570</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>49274173</v>
@@ -678,22 +678,22 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B12">
-        <v>27079012</v>
+        <v>34539596</v>
       </c>
       <c r="C12">
-        <v>2821171</v>
+        <v>4412670</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>29900183</v>
+        <v>38952266</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>84707882</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>915551972</v>
@@ -723,22 +723,22 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B15">
-        <v>38423840</v>
+        <v>30694157</v>
       </c>
       <c r="C15">
-        <v>3171080</v>
+        <v>1274302</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>41594920</v>
+        <v>31968459</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>7142279</v>
@@ -753,7 +753,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17">
         <v>61125130</v>
@@ -776,7 +776,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,99 +787,99 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>